<commit_message>
updates, not sure really
</commit_message>
<xml_diff>
--- a/Canbus Decode.xlsx
+++ b/Canbus Decode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marcellatwin/Documents/GitHub/honda-canbus-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC7D02-BCB4-8648-B128-EDBC2D0D97C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A944CD52-1DE3-CB44-B725-E15CF01E10BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1795,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>

</xml_diff>